<commit_message>
Version 1.51. Update rvf plug-in according to Plos ONE source code.
</commit_message>
<xml_diff>
--- a/recipes/student_projects/rvf/interactions.xlsx
+++ b/recipes/student_projects/rvf/interactions.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="19440" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -397,7 +397,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>